<commit_message>
Updated some component values.
</commit_message>
<xml_diff>
--- a/PCB/CAM_OUTPUTS/BOM/FLEXI_HAL_2000_CAM_OUTPUT_A5.xlsx
+++ b/PCB/CAM_OUTPUTS/BOM/FLEXI_HAL_2000_CAM_OUTPUT_A5.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\Flexi-HAL\PCB\CAM_OUTPUTS\A5_package\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\Flexi-HAL\PCB\CAM_OUTPUTS\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32145" windowHeight="15255"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32150" windowHeight="15260"/>
   </bookViews>
   <sheets>
     <sheet name="FLEXI_HAL_2000_CAM_OUTPUT_A5" sheetId="1" r:id="rId1"/>
@@ -620,9 +620,6 @@
     <t>Header 2</t>
   </si>
   <si>
-    <t>P16</t>
-  </si>
-  <si>
     <t>HDR1X2</t>
   </si>
   <si>
@@ -887,12 +884,6 @@
     <t>Dual Channel Isolator</t>
   </si>
   <si>
-    <t>C476471</t>
-  </si>
-  <si>
-    <t>CBMuD1200HAS8</t>
-  </si>
-  <si>
     <t>U9, U12, U13, U15, U16, U17, U29, U31, U33</t>
   </si>
   <si>
@@ -1065,6 +1056,15 @@
   </si>
   <si>
     <t>C22966</t>
+  </si>
+  <si>
+    <t>P1, P16, P20</t>
+  </si>
+  <si>
+    <t>CBMuD1200LAS8</t>
+  </si>
+  <si>
+    <t>C476470</t>
   </si>
 </sst>
 </file>
@@ -1409,23 +1409,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="8" width="19.7109375" customWidth="1"/>
-    <col min="9" max="9" width="33.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.54296875" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
+    <col min="3" max="3" width="34.453125" customWidth="1"/>
+    <col min="4" max="4" width="19.7265625" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" customWidth="1"/>
+    <col min="7" max="8" width="19.7265625" customWidth="1"/>
+    <col min="9" max="9" width="33.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>42</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>8</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>9</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>2</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>2</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>7</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>1</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>2</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>2</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>2</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>2</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>4</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>2</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>12</v>
       </c>
@@ -2181,13 +2181,13 @@
         <v>134</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>135</v>
@@ -2196,7 +2196,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>1</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>3</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>1</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>1</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>2</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>1</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>10</v>
       </c>
@@ -2360,13 +2360,13 @@
         <v>171</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>172</v>
@@ -2375,7 +2375,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>2</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>1</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>2</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>1</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>1</v>
       </c>
@@ -2496,509 +2496,509 @@
         <v>196</v>
       </c>
       <c r="H41" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="I41" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="I41" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>2</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>200</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="H42" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="I42" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="I42" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>5</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>205</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H43" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="I43" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="I43" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>3</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>209</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>115</v>
       </c>
       <c r="G44" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="H44" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>211</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>4</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>213</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>115</v>
       </c>
       <c r="G45" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="H45" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="H45" s="2" t="s">
+      <c r="I45" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="I45" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>7</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="G46" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="H46" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="H46" s="2" t="s">
-        <v>221</v>
-      </c>
       <c r="I46" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>5</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G47" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="H47" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="I47" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="I47" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>7</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G48" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="H48" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="H48" s="2" t="s">
-        <v>229</v>
-      </c>
       <c r="I48" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>23</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G49" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="H49" s="2" t="s">
-        <v>232</v>
-      </c>
       <c r="I49" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>4</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G50" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="H50" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="H50" s="2" t="s">
-        <v>235</v>
-      </c>
       <c r="I50" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>31</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G51" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="H51" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="H51" s="2" t="s">
-        <v>238</v>
-      </c>
       <c r="I51" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>16</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G52" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="H52" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H52" s="2" t="s">
-        <v>241</v>
-      </c>
       <c r="I52" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>10</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>5</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G54" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="H54" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="H54" s="2" t="s">
-        <v>246</v>
-      </c>
       <c r="I54" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>1</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G55" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="H55" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="H55" s="2" t="s">
-        <v>249</v>
-      </c>
       <c r="I55" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>1</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G56" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H56" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="H56" s="2" t="s">
-        <v>252</v>
-      </c>
       <c r="I56" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>1</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>2</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G58" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="H58" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="H58" s="2" t="s">
-        <v>255</v>
-      </c>
       <c r="I58" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>1</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G59" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="H59" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="H59" s="2" t="s">
-        <v>258</v>
-      </c>
       <c r="I59" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>1</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G60" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="H60" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="H60" s="2" t="s">
-        <v>261</v>
-      </c>
       <c r="I60" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>3</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G61" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="H61" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="H61" s="2" t="s">
-        <v>264</v>
-      </c>
       <c r="I61" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>2</v>
       </c>
@@ -3006,86 +3006,86 @@
         <v>15</v>
       </c>
       <c r="C62" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>267</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G62" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="H62" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="H62" s="2" t="s">
+      <c r="I62" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="I62" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>21</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="E63" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="F63" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="G63" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="G63" s="2" t="s">
+      <c r="H63" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="H63" s="2" t="s">
-        <v>277</v>
-      </c>
       <c r="I63" s="2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>1</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="E64" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="F64" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="F64" s="2" t="s">
+      <c r="G64" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="H64" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="G64" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="H64" s="2" t="s">
+      <c r="I64" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="I64" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>9</v>
       </c>
@@ -3096,255 +3096,255 @@
         <v>15</v>
       </c>
       <c r="D65" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="H65" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="E65" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="I65" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>1</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="G66" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="H66" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="F66" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>293</v>
-      </c>
       <c r="I66" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>1</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="H67" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="E67" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>297</v>
-      </c>
       <c r="I67" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>3</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E68" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="F68" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="G68" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="H68" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="E68" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>303</v>
-      </c>
       <c r="I68" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>1</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E69" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="F69" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="G69" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="H69" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="I69" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="F69" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="I69" s="2" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>1</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="H70" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="E70" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>314</v>
-      </c>
       <c r="I70" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>1</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>1</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="G72" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="H72" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="F72" s="2" t="s">
+      <c r="I72" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="G72" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="H72" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="I72" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>1</v>
       </c>
       <c r="B73" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E73" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="F73" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="G73" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="H73" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="E73" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>331</v>
-      </c>
       <c r="I73" s="2" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>1</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>